<commit_message>
fix translate issue, add one instance lock
</commit_message>
<xml_diff>
--- a/server/corelib/lang/all_lang_V1.6.xlsx
+++ b/server/corelib/lang/all_lang_V1.6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\digiCenter\server\corelib\lang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B267681-F539-4EB4-A7A6-6DFCEE63D0A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{196385F2-1D96-4B7B-99AB-93A15ADCFD41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="1089">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1285" uniqueCount="1173">
   <si>
     <t>name</t>
   </si>
@@ -3578,6 +3578,304 @@
   </si>
   <si>
     <t>详细错误描述</t>
+  </si>
+  <si>
+    <t>general_digitest_mode_switch</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Force Manual Mode</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>啟用手動測試模式</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kraft Manueller Modus</t>
+  </si>
+  <si>
+    <t>启用手动测试模式</t>
+  </si>
+  <si>
+    <t>report_groupTable_tab</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Group Table</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>分組表格</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gruppentabelle</t>
+  </si>
+  <si>
+    <t>分组表格</t>
+  </si>
+  <si>
+    <t>target_temperature</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>target temperature</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>tolerance</t>
+  </si>
+  <si>
+    <t>slope</t>
+  </si>
+  <si>
+    <t>increment</t>
+  </si>
+  <si>
+    <t>mode</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>method</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>measuring time</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>number of measurement</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>numerical method</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>loop id</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>loop counts</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>loop color</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>stop on</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>measuring_time</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>number_of_measurement</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>numerical_method</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>目標溫度</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>容許範圍</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>溫升斜率</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>溫度增幅(需搭配迴圈)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>increment(valid only inside the loop)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>模式</t>
+  </si>
+  <si>
+    <t>模式</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>方法</t>
+  </si>
+  <si>
+    <t>方法</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>量測時間</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>量測次數</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>輸出數值算法</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>conditioning time</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>conditioning_time</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>等待時間</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>迴圈辨別號</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>迴圈次數</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>迴圈顏色</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>停止條件</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zieltemperatur</t>
+  </si>
+  <si>
+    <t>目标温度</t>
+  </si>
+  <si>
+    <t>Toleranz</t>
+  </si>
+  <si>
+    <t>容许范围</t>
+  </si>
+  <si>
+    <t>Steigung</t>
+  </si>
+  <si>
+    <t>温升斜率</t>
+  </si>
+  <si>
+    <t>increment (gilt nur innerhalb der Schleife)</t>
+  </si>
+  <si>
+    <t>温度增幅(需搭配回圈)</t>
+  </si>
+  <si>
+    <t>Modus</t>
+  </si>
+  <si>
+    <t>Methode</t>
+  </si>
+  <si>
+    <t>Messzeit</t>
+  </si>
+  <si>
+    <t>量测时间</t>
+  </si>
+  <si>
+    <t>Anzahl der Mess</t>
+  </si>
+  <si>
+    <t>量测次数</t>
+  </si>
+  <si>
+    <t>numerische Methode</t>
+  </si>
+  <si>
+    <t>输出数值算法</t>
+  </si>
+  <si>
+    <t>Konditionierungszeit</t>
+  </si>
+  <si>
+    <t>等待时间</t>
+  </si>
+  <si>
+    <t>loop id</t>
+  </si>
+  <si>
+    <t>回圈辨别号</t>
+  </si>
+  <si>
+    <t>Schleifenzählungen</t>
+  </si>
+  <si>
+    <t>回圈次数</t>
+  </si>
+  <si>
+    <t>Loop-Farb</t>
+  </si>
+  <si>
+    <t>回圈颜色</t>
+  </si>
+  <si>
+    <t>Aufhören</t>
+  </si>
+  <si>
+    <t>停止条件</t>
+  </si>
+  <si>
+    <t>loopid</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>loop_counts</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>loop_color</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>waiting_time</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>safe_temperature</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>waiting time</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>safe temperature</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>等待時間</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>安全溫度</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wartezeit</t>
+  </si>
+  <si>
+    <t>sichere Temperatur</t>
+  </si>
+  <si>
+    <t>安全温度</t>
   </si>
 </sst>
 </file>
@@ -3680,7 +3978,37 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="52">
+  <dxfs count="55">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4535,10 +4863,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F239"/>
+  <dimension ref="A1:F257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A221" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E246" sqref="E246"/>
+    <sheetView tabSelected="1" topLeftCell="A230" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C253" sqref="C253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -9326,264 +9654,639 @@
         <v>1088</v>
       </c>
     </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A240" s="2">
+        <v>236</v>
+      </c>
+      <c r="B240" s="1" t="s">
+        <v>1089</v>
+      </c>
+      <c r="C240" s="1" t="s">
+        <v>1090</v>
+      </c>
+      <c r="D240" s="1" t="s">
+        <v>1091</v>
+      </c>
+      <c r="E240" s="1" t="s">
+        <v>1092</v>
+      </c>
+      <c r="F240" s="1" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A241" s="2">
+        <v>237</v>
+      </c>
+      <c r="B241" s="1" t="s">
+        <v>1094</v>
+      </c>
+      <c r="C241" s="1" t="s">
+        <v>1095</v>
+      </c>
+      <c r="D241" s="1" t="s">
+        <v>1096</v>
+      </c>
+      <c r="E241" s="1" t="s">
+        <v>1097</v>
+      </c>
+      <c r="F241" s="1" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A242" s="2">
+        <v>238</v>
+      </c>
+      <c r="B242" s="1" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C242" s="1" t="s">
+        <v>1100</v>
+      </c>
+      <c r="D242" s="1" t="s">
+        <v>1116</v>
+      </c>
+      <c r="E242" s="1" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F242" s="1" t="s">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A243" s="2">
+        <v>239</v>
+      </c>
+      <c r="B243" s="1" t="s">
+        <v>1101</v>
+      </c>
+      <c r="C243" s="1" t="s">
+        <v>1101</v>
+      </c>
+      <c r="D243" s="1" t="s">
+        <v>1117</v>
+      </c>
+      <c r="E243" s="1" t="s">
+        <v>1137</v>
+      </c>
+      <c r="F243" s="1" t="s">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A244" s="2">
+        <v>240</v>
+      </c>
+      <c r="B244" s="1" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C244" s="1" t="s">
+        <v>1102</v>
+      </c>
+      <c r="D244" s="1" t="s">
+        <v>1118</v>
+      </c>
+      <c r="E244" s="1" t="s">
+        <v>1139</v>
+      </c>
+      <c r="F244" s="1" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A245" s="2">
+        <v>241</v>
+      </c>
+      <c r="B245" s="1" t="s">
+        <v>1103</v>
+      </c>
+      <c r="C245" s="1" t="s">
+        <v>1120</v>
+      </c>
+      <c r="D245" s="1" t="s">
+        <v>1119</v>
+      </c>
+      <c r="E245" s="1" t="s">
+        <v>1141</v>
+      </c>
+      <c r="F245" s="1" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A246" s="2">
+        <v>242</v>
+      </c>
+      <c r="B246" s="1" t="s">
+        <v>1104</v>
+      </c>
+      <c r="C246" s="1" t="s">
+        <v>1104</v>
+      </c>
+      <c r="D246" s="1" t="s">
+        <v>1122</v>
+      </c>
+      <c r="E246" s="1" t="s">
+        <v>1143</v>
+      </c>
+      <c r="F246" s="1" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A247" s="2">
+        <v>243</v>
+      </c>
+      <c r="B247" s="1" t="s">
+        <v>1105</v>
+      </c>
+      <c r="C247" s="1" t="s">
+        <v>1105</v>
+      </c>
+      <c r="D247" s="1" t="s">
+        <v>1124</v>
+      </c>
+      <c r="E247" s="1" t="s">
+        <v>1144</v>
+      </c>
+      <c r="F247" s="1" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A248" s="2">
+        <v>244</v>
+      </c>
+      <c r="B248" s="1" t="s">
+        <v>1113</v>
+      </c>
+      <c r="C248" s="1" t="s">
+        <v>1106</v>
+      </c>
+      <c r="D248" s="1" t="s">
+        <v>1125</v>
+      </c>
+      <c r="E248" s="1" t="s">
+        <v>1145</v>
+      </c>
+      <c r="F248" s="1" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A249" s="2">
+        <v>245</v>
+      </c>
+      <c r="B249" s="1" t="s">
+        <v>1114</v>
+      </c>
+      <c r="C249" s="1" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D249" s="1" t="s">
+        <v>1126</v>
+      </c>
+      <c r="E249" s="1" t="s">
+        <v>1147</v>
+      </c>
+      <c r="F249" s="1" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A250" s="2">
+        <v>246</v>
+      </c>
+      <c r="B250" s="1" t="s">
+        <v>1115</v>
+      </c>
+      <c r="C250" s="1" t="s">
+        <v>1108</v>
+      </c>
+      <c r="D250" s="1" t="s">
+        <v>1127</v>
+      </c>
+      <c r="E250" s="1" t="s">
+        <v>1149</v>
+      </c>
+      <c r="F250" s="1" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A251" s="2">
+        <v>247</v>
+      </c>
+      <c r="B251" s="1" t="s">
+        <v>1129</v>
+      </c>
+      <c r="C251" s="1" t="s">
+        <v>1128</v>
+      </c>
+      <c r="D251" s="1" t="s">
+        <v>1130</v>
+      </c>
+      <c r="E251" s="1" t="s">
+        <v>1151</v>
+      </c>
+      <c r="F251" s="1" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A252" s="2">
+        <v>248</v>
+      </c>
+      <c r="B252" s="1" t="s">
+        <v>1161</v>
+      </c>
+      <c r="C252" s="1" t="s">
+        <v>1109</v>
+      </c>
+      <c r="D252" s="1" t="s">
+        <v>1131</v>
+      </c>
+      <c r="E252" s="1" t="s">
+        <v>1153</v>
+      </c>
+      <c r="F252" s="1" t="s">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A253" s="2">
+        <v>249</v>
+      </c>
+      <c r="B253" s="1" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C253" s="1" t="s">
+        <v>1110</v>
+      </c>
+      <c r="D253" s="1" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E253" s="1" t="s">
+        <v>1155</v>
+      </c>
+      <c r="F253" s="1" t="s">
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A254" s="2">
+        <v>250</v>
+      </c>
+      <c r="B254" s="1" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C254" s="1" t="s">
+        <v>1111</v>
+      </c>
+      <c r="D254" s="1" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E254" s="1" t="s">
+        <v>1157</v>
+      </c>
+      <c r="F254" s="1" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A255" s="2">
+        <v>251</v>
+      </c>
+      <c r="B255" s="1" t="s">
+        <v>1112</v>
+      </c>
+      <c r="C255" s="1" t="s">
+        <v>1112</v>
+      </c>
+      <c r="D255" s="1" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E255" s="1" t="s">
+        <v>1159</v>
+      </c>
+      <c r="F255" s="1" t="s">
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A256" s="2">
+        <v>252</v>
+      </c>
+      <c r="B256" s="1" t="s">
+        <v>1164</v>
+      </c>
+      <c r="C256" s="1" t="s">
+        <v>1166</v>
+      </c>
+      <c r="D256" s="6" t="s">
+        <v>1168</v>
+      </c>
+      <c r="E256" s="1" t="s">
+        <v>1170</v>
+      </c>
+      <c r="F256" s="1" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A257" s="2">
+        <v>253</v>
+      </c>
+      <c r="B257" s="1" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C257" s="1" t="s">
+        <v>1167</v>
+      </c>
+      <c r="D257" s="1" t="s">
+        <v>1169</v>
+      </c>
+      <c r="E257" s="1" t="s">
+        <v>1171</v>
+      </c>
+      <c r="F257" s="1" t="s">
+        <v>1172</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="B168:E169 B1:E3 B154:E166 B97:E152 B69:E72 B5:E15 B17:E66 B179:E207 B211:E211 B214:E1048576 B75:E89">
+  <conditionalFormatting sqref="B168:E169 B1:E3 B154:E166 B97:E152 B69:E72 B5:E15 B17:E66 B179:E207 B211:E211 B214:E241 B75:E89 B257:E1048576 D252:E256 C242:E251">
+    <cfRule type="cellIs" dxfId="54" priority="57" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B167:E167">
+    <cfRule type="cellIs" dxfId="53" priority="56" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B171:E172">
+    <cfRule type="cellIs" dxfId="52" priority="55" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B153:E153">
     <cfRule type="cellIs" dxfId="51" priority="54" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B167:E167">
+  <conditionalFormatting sqref="B173:E173 B174 D174:E174">
     <cfRule type="cellIs" dxfId="50" priority="53" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B171:E172">
+  <conditionalFormatting sqref="B175:E175 B176 D176:E176">
     <cfRule type="cellIs" dxfId="49" priority="52" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B153:E153">
+  <conditionalFormatting sqref="B177:E178">
     <cfRule type="cellIs" dxfId="48" priority="51" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B173:E173 B174 D174:E174">
+  <conditionalFormatting sqref="C176">
     <cfRule type="cellIs" dxfId="47" priority="50" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B175:E175 B176 D176:E176">
+  <conditionalFormatting sqref="C174">
     <cfRule type="cellIs" dxfId="46" priority="49" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B177:E178">
+  <conditionalFormatting sqref="B90:E90">
     <cfRule type="cellIs" dxfId="45" priority="48" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C176">
+  <conditionalFormatting sqref="B91:D93">
     <cfRule type="cellIs" dxfId="44" priority="47" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C174">
+  <conditionalFormatting sqref="E91:E92">
     <cfRule type="cellIs" dxfId="43" priority="46" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B90:E90">
+  <conditionalFormatting sqref="B94:D94 B96:D96">
     <cfRule type="cellIs" dxfId="42" priority="45" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B91:D93">
+  <conditionalFormatting sqref="E94 E96">
     <cfRule type="cellIs" dxfId="41" priority="44" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E91:E92">
+  <conditionalFormatting sqref="B4:E4">
     <cfRule type="cellIs" dxfId="40" priority="43" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B94:D94 B96:D96">
+  <conditionalFormatting sqref="B67:E68">
     <cfRule type="cellIs" dxfId="39" priority="42" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E94 E96">
+  <conditionalFormatting sqref="B208:E209">
     <cfRule type="cellIs" dxfId="38" priority="41" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4:E4">
+  <conditionalFormatting sqref="B73:D74">
     <cfRule type="cellIs" dxfId="37" priority="40" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B67:E68">
+  <conditionalFormatting sqref="E74">
     <cfRule type="cellIs" dxfId="36" priority="39" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B208:E209">
+  <conditionalFormatting sqref="E73">
     <cfRule type="cellIs" dxfId="35" priority="38" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B73:D74">
+  <conditionalFormatting sqref="B16:E16">
     <cfRule type="cellIs" dxfId="34" priority="37" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E74">
+  <conditionalFormatting sqref="E93">
     <cfRule type="cellIs" dxfId="33" priority="36" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E73">
+  <conditionalFormatting sqref="B207:E207">
     <cfRule type="cellIs" dxfId="32" priority="35" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B16:E16">
+  <conditionalFormatting sqref="B206:E206">
     <cfRule type="cellIs" dxfId="31" priority="34" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E93">
+  <conditionalFormatting sqref="F168:F169 F1:F3 F154:F166 F97:F152 F69:F72 F5:F15 F75:F89 F17:F66 F179:F207 F211 F214:F1048576">
     <cfRule type="cellIs" dxfId="30" priority="33" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B207:E207">
+  <conditionalFormatting sqref="F167">
     <cfRule type="cellIs" dxfId="29" priority="32" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B206:E206">
+  <conditionalFormatting sqref="F171:F172">
     <cfRule type="cellIs" dxfId="28" priority="31" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F168:F169 F1:F3 F154:F166 F97:F152 F69:F72 F5:F15 F75:F89 F17:F66 F179:F207 F211 F214:F1048576">
+  <conditionalFormatting sqref="F153">
     <cfRule type="cellIs" dxfId="27" priority="30" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F167">
+  <conditionalFormatting sqref="F173:F174">
     <cfRule type="cellIs" dxfId="26" priority="29" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F171:F172">
+  <conditionalFormatting sqref="F175:F176">
     <cfRule type="cellIs" dxfId="25" priority="28" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F153">
+  <conditionalFormatting sqref="F177:F178">
     <cfRule type="cellIs" dxfId="24" priority="27" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F173:F174">
+  <conditionalFormatting sqref="F90">
     <cfRule type="cellIs" dxfId="23" priority="26" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F175:F176">
+  <conditionalFormatting sqref="F91:F93">
     <cfRule type="cellIs" dxfId="22" priority="25" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F177:F178">
+  <conditionalFormatting sqref="F94 F96">
     <cfRule type="cellIs" dxfId="21" priority="24" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F90">
+  <conditionalFormatting sqref="F4">
     <cfRule type="cellIs" dxfId="20" priority="23" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F91:F93">
+  <conditionalFormatting sqref="F67:F68">
     <cfRule type="cellIs" dxfId="19" priority="22" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F94 F96">
+  <conditionalFormatting sqref="F208:F209">
     <cfRule type="cellIs" dxfId="18" priority="21" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F4">
+  <conditionalFormatting sqref="F73:F74">
     <cfRule type="cellIs" dxfId="17" priority="20" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F67:F68">
+  <conditionalFormatting sqref="F16">
     <cfRule type="cellIs" dxfId="16" priority="19" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F208:F209">
+  <conditionalFormatting sqref="F207">
     <cfRule type="cellIs" dxfId="15" priority="18" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F73:F74">
+  <conditionalFormatting sqref="F206">
     <cfRule type="cellIs" dxfId="14" priority="17" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F16">
-    <cfRule type="cellIs" dxfId="13" priority="16" operator="equal">
-      <formula>"TBD"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F207">
-    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
-      <formula>"TBD"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F206">
-    <cfRule type="cellIs" dxfId="11" priority="14" operator="equal">
-      <formula>"TBD"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B212:E212">
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F212">
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B210:E210">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F210">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B170:E170">
     <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B210:E210">
+  <conditionalFormatting sqref="F170">
     <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F210">
+  <conditionalFormatting sqref="B95:D95">
     <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B170:E170">
+  <conditionalFormatting sqref="E95">
     <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F170">
+  <conditionalFormatting sqref="F95">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B95:D95">
+  <conditionalFormatting sqref="B213:E213">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E95">
+  <conditionalFormatting sqref="F213">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F95">
+  <conditionalFormatting sqref="C252:C256">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B213:E213">
+  <conditionalFormatting sqref="B242:B251">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F213">
+  <conditionalFormatting sqref="B252:B256">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>

</xml_diff>